<commit_message>
make excel view better
</commit_message>
<xml_diff>
--- a/check_script/requirements.xlsx
+++ b/check_script/requirements.xlsx
@@ -34,12 +34,6 @@
     <t>mode</t>
   </si>
   <si>
-    <t>Android_version</t>
-  </si>
-  <si>
-    <t>Memory</t>
-  </si>
-  <si>
     <t>requirements</t>
   </si>
   <si>
@@ -47,6 +41,12 @@
   </si>
   <si>
     <t>satisfy</t>
+  </si>
+  <si>
+    <t>Android_version</t>
+  </si>
+  <si>
+    <t>Memory</t>
   </si>
 </sst>
 </file>
@@ -983,48 +983,46 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="B3" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some function and pack functions
</commit_message>
<xml_diff>
--- a/check_script/requirements.xlsx
+++ b/check_script/requirements.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>mode</t>
   </si>
@@ -46,7 +46,34 @@
     <t>Android_version</t>
   </si>
   <si>
+    <t>Kernel_version</t>
+  </si>
+  <si>
+    <t>6.6.50</t>
+  </si>
+  <si>
+    <t>User_version</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
     <t>Memory</t>
+  </si>
+  <si>
+    <t>CPU_kernel_count</t>
+  </si>
+  <si>
+    <t>CPU_load_1min</t>
+  </si>
+  <si>
+    <t>CPU_load_5min</t>
+  </si>
+  <si>
+    <t>CPU_load_15min</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -983,16 +1010,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
@@ -1010,19 +1037,75 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>23.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update some functions include lmk, readahead, writeback, ioscheduler compare
</commit_message>
<xml_diff>
--- a/check_script/requirements.xlsx
+++ b/check_script/requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="27915" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>mode</t>
   </si>
@@ -43,6 +43,9 @@
     <t>satisfy</t>
   </si>
   <si>
+    <t>device</t>
+  </si>
+  <si>
     <t>Android_version</t>
   </si>
   <si>
@@ -59,6 +62,27 @@
   </si>
   <si>
     <t>Memory</t>
+  </si>
+  <si>
+    <t>lmk_minfree_levels</t>
+  </si>
+  <si>
+    <t>dirty_ratio</t>
+  </si>
+  <si>
+    <t>dirty_background_ratio</t>
+  </si>
+  <si>
+    <t>readahead</t>
+  </si>
+  <si>
+    <t>sda</t>
+  </si>
+  <si>
+    <t>io_scheduler</t>
+  </si>
+  <si>
+    <t>cfp</t>
   </si>
   <si>
     <t>CPU_kernel_count</t>
@@ -689,12 +713,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1010,19 +1031,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
     <col min="2" max="2" width="17.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,10 +1056,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>14</v>
@@ -1046,65 +1070,111 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1024</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
         <v>23.5</v>
       </c>
     </row>

</xml_diff>